<commit_message>
#887 removed unwanted columns
</commit_message>
<xml_diff>
--- a/RPGSmithApp/RPGSmithApp/ClientApp/src/app/assets/template/SampleMonsterTemplates.xlsx
+++ b/RPGSmithApp/RPGSmithApp/ClientApp/src/app/assets/template/SampleMonsterTemplates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="327" yWindow="524" windowWidth="13235" windowHeight="4451"/>
+    <workbookView xWindow="327" yWindow="524" windowWidth="13235" windowHeight="4451" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterTemplates" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
-  <si>
-    <t>monsterTemplateId</t>
-  </si>
-  <si>
-    <t>ruleSetId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -50,12 +44,6 @@
     <t>metatags</t>
   </si>
   <si>
-    <t>parentMonsterTemplateId</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
     <t>health</t>
   </si>
   <si>
@@ -71,34 +59,7 @@
     <t>initiativeCommand</t>
   </si>
   <si>
-    <t>isRandomizationEngine</t>
-  </si>
-  <si>
     <t>gmOnly</t>
-  </si>
-  <si>
-    <t>parentMonsterTemplate</t>
-  </si>
-  <si>
-    <t>ruleSet</t>
-  </si>
-  <si>
-    <t>monsterTemplateCommands</t>
-  </si>
-  <si>
-    <t>monsterTemplateAbilities</t>
-  </si>
-  <si>
-    <t>monsterTemplateSpells</t>
-  </si>
-  <si>
-    <t>monsterTemplateBuffAndEffects</t>
-  </si>
-  <si>
-    <t>monsterTemplateItemMasters</t>
-  </si>
-  <si>
-    <t>monsterTemplateMonsters</t>
   </si>
   <si>
     <t>abilityId</t>
@@ -506,34 +467,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,287 +523,185 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75"/>
-    <row r="3" spans="1:26" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75"/>
-    <row r="3" spans="1:3" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75"/>
-    <row r="3" spans="1:3" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75"/>
-    <row r="3" spans="1:3" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 B1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:D1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 B1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75"/>
-    <row r="3" spans="1:5" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
-  <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -864,41 +712,33 @@
     <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>